<commit_message>
add NullArrayException and annotations to time test graphs
</commit_message>
<xml_diff>
--- a/complexity/complexity.xlsx
+++ b/complexity/complexity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekty\Studia\ASTRUK\sorting-algorithms\complexity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE497DC-6E17-436D-932A-CB89CA1A7B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F536785F-FE5E-4544-9B3E-2778833A7296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4B1DEF79-769B-154A-8BD5-F1EBB54A2C6C}"/>
   </bookViews>
@@ -214,7 +214,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.4203876988086609E-2"/>
+          <c:y val="0.10505324289945375"/>
+          <c:w val="0.86410808731682931"/>
+          <c:h val="0.75602347722855923"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1161,6 +1171,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -5751,6 +5762,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -8465,6 +8477,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -10509,6 +10522,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -12206,6 +12220,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -22802,7 +22817,679 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>530086</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>157370</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4050195" cy="2503506"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="pole tekstowe 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B1B9B9-DE35-4482-9491-6A93E55C2D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1217543" y="4729370"/>
+          <a:ext cx="4050195" cy="2503506"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>W najlepszym</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> przypadku (tablica już posortowana) złożoność</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>sortowania przez wstawianie wynosi O(n) a więc czas sortowania</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>rośnie liniowo.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>Początek tego wykresu pokazuje wzrost liniowy, lecz w okolicy n=12000 drastycznie spada czas sortowania, podejrzewam że jest</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>to spowodowane automatyczną optymalizacją często powtarzanych</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>operacji przez procesor. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>Do n=70000 przebieg jest z grubsza liniowy,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>lecz reszta przebiegu, chociaż dalej przejawia swoją liniowość, to występują duże szpikulce w czasie sortowania. Podejrzewam że jest to spowodowane walką o zasoby procesora przez inne procesy, szczególnie że w tym momencie tablica double[70000] osiąga już</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>rozmiar &gt;0,5 megabajta, czyli więcej niż 1/16 pamięci podręcznej</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>procesora w moim komputerze [Intel Core i7-4770K]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>140805</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>74544</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5387565" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="pole tekstowe 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C3A0A03-B967-4B77-BB1D-A93C8F5856E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17327218" y="869674"/>
+          <a:ext cx="5387565" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Sortowanie szybkie ma w najgorszym wypadku (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>wszystkie wartości w tablicy są takie same,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>w efekcie pivot zawsze jest wartością największą/najmniejszą) złożoność O(n^2).</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>136070</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8382000" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="pole tekstowe 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97750B2-728D-4121-808F-8F63E89FF2F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7320643" y="17485177"/>
+          <a:ext cx="8382000" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Mimo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> że sortowanie szybkie jest w każdej sytuacji szybsze niż sortowanie przez wybieranie, to sortowanie przez wstawianie wystaje. Dla najgorszych przypadków zajmuje ono dłużej niż pozostałe, chociaz pozostająć w ich niedalekiej okolicy, to dla przypadków optymistycznych jest ono drastycznie szybsze niż pozostałe.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.88253</cdr:x>
+      <cdr:y>0.05228</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.26784</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A92D699F-6853-46CC-BAC2-2758B354DEFF}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7072234" y="221796"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.12543</cdr:x>
+      <cdr:y>0.17777</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.67891</cdr:x>
+      <cdr:y>0.36381</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="pole tekstowe 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99D616F0-29AE-48BF-B5B9-C06856AE1479}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="986120" y="734216"/>
+          <a:ext cx="4351500" cy="768412"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Złożoność</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> sortowania przez wstawianie w najgorszym wypadku </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>(tablica posortowana w odwrotnej kolejności) osiąga O(n^2), i wykres ten </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>obrazuje wykładniczą nature złożoności dla coraz większego n.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19534</cdr:x>
+      <cdr:y>0.22871</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.63062</cdr:x>
+      <cdr:y>0.43721</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="pole tekstowe 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{570972F4-88DC-412C-A22D-677FB747366A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1520519" y="970189"/>
+          <a:ext cx="3388179" cy="884465"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16931</cdr:x>
+      <cdr:y>0.15804</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.6792</cdr:x>
+      <cdr:y>0.29641</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{920BACF9-1F40-45ED-AF10-2E3530B57102}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1331104" y="652742"/>
+          <a:ext cx="4008783" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Sortowanie</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> przez wybieranie ma stałą złożoność wynoszącą O(n^2),</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>i jej wykładnicza natura jest odwzorowana na tym wykresie.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.26103</cdr:x>
+      <cdr:y>0.56836</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.77619</cdr:x>
+      <cdr:y>0.71042</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541C0CFD-7176-4C7F-BB4F-53D6DBF50067}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2052189" y="2352903"/>
+          <a:ext cx="4050195" cy="588065"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Zgodnie z oczekiwaniami,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> czas sortowania dla przypadku </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>najlepszego jest znacznie mniejszy niż dla przypadku najgorszego.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16816</cdr:x>
+      <cdr:y>0.17777</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.61198</cdr:x>
+      <cdr:y>0.28004</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF103BB-A48F-4908-AA74-62EA06FC853A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1321161" y="734218"/>
+          <a:ext cx="3486979" cy="422413"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16605</cdr:x>
+      <cdr:y>0.24194</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.28243</cdr:x>
+      <cdr:y>0.52068</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="pole tekstowe 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5441FB-280B-4277-920F-13048315CD45}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1304597" y="999261"/>
+          <a:ext cx="914400" cy="1151283"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>W najlepszym</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> przypadku (tablica już posortowana,w efekcie </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>pivot zawsze jest medianą) sortowanie szybkie ma złożoność O(n*log(n)).</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pl-PL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>Chwilowe wzrosty czasu sortowania pod koniec przebiegu funkcji są prawdopodobnie</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>spowodowane innymi procesami na komputerze w trakcie prowadzenia testów</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>czasowych.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.17924</cdr:x>
+      <cdr:y>0.17301</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.29562</cdr:x>
+      <cdr:y>0.3944</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F106C6-8716-4534-8AB1-31F9D46D3494}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1408239" y="714579"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Jak widać czas</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> sortowania w przypadku pesymistycznym wzrasta</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>znacznie szybciej niż w przypadku optymistycznym.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26402,8 +27089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E41AAB0-3D41-4D74-ABE5-06ACE5804688}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="BO12" sqref="BO12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>